<commit_message>
Create plots to visualise the R-gene clusters.
</commit_message>
<xml_diff>
--- a/Tests/PlantExp data/seedlings/T.test_compare_enrichment_between_R-genes_at_each_expression_level.xlsx
+++ b/Tests/PlantExp data/seedlings/T.test_compare_enrichment_between_R-genes_at_each_expression_level.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/42a5ee813758fc42/Documents/PhD/PhD.git/Tests/PlantExp data/seedlings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B3CDB77-2DD3-4A3A-BE1A-95F0BCF72425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{0B3CDB77-2DD3-4A3A-BE1A-95F0BCF72425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7F5A16E3-6102-45D2-8C99-38400C475306}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T.test_compare_enrichment_betwe" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -451,7 +451,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -566,6 +566,123 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -611,9 +728,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -968,11 +1097,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E171"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A143" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162:E171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,2909 +1114,2909 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>-1.5757517312501299</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>0.117280655579723</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="8">
         <v>2.18970125312363</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="8">
         <v>3.1082235275389399E-2</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
         <v>2.0450152738813698</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>4.3891424895043697E-2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="8">
         <v>3.1439331614885702</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
         <v>2.19335779661314E-3</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="8">
         <v>-1.57612887076587</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="8">
         <v>0.117675668366238</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>-2.7428635993492798</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <v>7.0687905837985799E-3</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <v>-3.0501687730957801</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <v>2.85417694437721E-3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
         <v>-2.4429700329737298</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>1.60356880715158E-2</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="8">
         <v>-2.59488700201985</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="8">
         <v>1.0537953971994999E-2</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="11">
         <v>-1.6340272525333599</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="11">
         <v>0.104463752037145</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>0.56431643116654095</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="5">
         <v>0.57381583698162497</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="8">
         <v>1.5397664576633301</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="8">
         <v>0.128852362859109</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="8">
         <v>1.6443344866315599</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="8">
         <v>0.10581173114386</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="8">
         <v>1.20512766523417</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="8">
         <v>0.232386244479273</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="8">
         <v>1.2975287528063999</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="8">
         <v>0.19854510278224599</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="8">
         <v>1.9324339577028</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="8">
         <v>5.84008557837691E-2</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="8">
         <v>1.2748635509484001</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="8">
         <v>0.20705397188528901</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="8">
         <v>0.97168016602121599</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="8">
         <v>0.334261433534282</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="8">
         <v>0.105270145176616</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="8">
         <v>0.91637119185089599</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="11">
         <v>-0.86930412068506402</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="11">
         <v>0.38610501120588298</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="5">
         <v>0.92672313608252399</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="5">
         <v>0.35632169641012801</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="A23" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="8">
         <v>4.6318719115555202</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="13">
         <v>1.5992036512431799E-5</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="8">
         <v>4.8147992940024604</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="13">
         <v>7.7119834422287293E-6</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="A25" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="8">
         <v>6.4497234313434797</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="13">
         <v>9.29588390162589E-9</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="A26" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="8">
         <v>5.0501026549309103</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="13">
         <v>2.6003097292290999E-6</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="8">
         <v>4.6059436839071903</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="13">
         <v>1.48578451242108E-5</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="8">
         <v>4.3338423155994601</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="13">
         <v>4.0221569225390598E-5</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E28" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="8">
         <v>4.4511587499027803</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="13">
         <v>2.7114825092428999E-5</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="A30" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="8">
         <v>2.8870566320987301</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="8">
         <v>4.9207738468133397E-3</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="A31" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="11">
         <v>2.4571616616791401</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="11">
         <v>1.63552064307062E-2</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="A32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="5">
         <v>-0.50624040160191297</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="5">
         <v>0.61354581623180304</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="A33" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="8">
         <v>0.65169673736079203</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="8">
         <v>0.51582959648017301</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="8">
         <v>1.2489216818373401</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="8">
         <v>0.213991262527851</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="8">
         <v>4.5966846261146701</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="13">
         <v>9.9767696513893896E-6</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="8">
         <v>4.4072919088313398</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="13">
         <v>2.5752651360102401E-5</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E36" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="8">
         <v>4.2509946083452803</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="13">
         <v>4.5434392499154698E-5</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E37" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="A38" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="8">
         <v>4.7049015546434898</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="13">
         <v>7.1495201457768398E-6</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="A39" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="8">
         <v>5.8916975817512602</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="13">
         <v>3.3857663226434697E-8</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="A40" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="8">
         <v>3.9385999094859301</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="8">
         <v>1.41568378064643E-4</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="11">
         <v>1.2919899548626399</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="11">
         <v>0.19944099140330401</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="5">
         <v>1.11104445758424</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="5">
         <v>0.26997009482676998</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="A43" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="8">
         <v>0.45412743526799798</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="8">
         <v>0.65064903416073905</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="A44" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="8">
         <v>0.87026778009636296</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="8">
         <v>0.38625090659184202</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="A45" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="8">
         <v>0.36114622458631501</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="8">
         <v>0.71866495247520201</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E45" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="A46" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="8">
         <v>-0.17492739235358201</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="8">
         <v>0.86146258566395295</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E46" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A47" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="8">
         <v>0.13007751678176399</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="8">
         <v>0.89673802499220501</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="A48" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="8">
         <v>1.3684269979480499</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="8">
         <v>0.17468779805446299</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="A49" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="8">
         <v>2.9741983847245899</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="8">
         <v>3.9686928272742398E-3</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="A50" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="8">
         <v>1.7314433113980601</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="8">
         <v>8.6671525124895205E-2</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="11">
         <v>0.98519960654812999</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="11">
         <v>0.32741010450494101</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="5">
         <v>-0.98874388392921098</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="5">
         <v>0.32444060489969501</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="A53" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="8">
         <v>-1.05396283771013</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="8">
         <v>0.29393519164553999</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="A54" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="8">
         <v>-1.5631839337319799</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="8">
         <v>0.12057832991685299</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="8">
         <v>-2.9447846690841102</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="8">
         <v>3.9663627270137003E-3</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="8">
         <v>-3.2744071681003399</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="8">
         <v>1.3660755481700599E-3</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="8">
         <v>-0.26872937562197202</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="8">
         <v>0.78863602242226105</v>
       </c>
-      <c r="E57" t="s">
+      <c r="E57" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="8">
         <v>2.0823372867310699</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="8">
         <v>3.9765678046095397E-2</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E58" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="8">
         <v>5.6979362932523099</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59" s="13">
         <v>2.1827135666671401E-7</v>
       </c>
-      <c r="E59" t="s">
+      <c r="E59" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="8">
         <v>1.2987494793549701</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="8">
         <v>0.19730897415277501</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E60" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+      <c r="A61" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="11">
         <v>-1.0760117317354301</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="11">
         <v>0.28398595586348402</v>
       </c>
-      <c r="E61" t="s">
+      <c r="E61" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+      <c r="A62" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="5">
         <v>-0.63628318401422501</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="5">
         <v>0.52584914703331398</v>
       </c>
-      <c r="E62" t="s">
+      <c r="E62" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+      <c r="A63" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="8">
         <v>-2.8876693266320799</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="8">
         <v>4.4515952129805204E-3</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+      <c r="A64" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="8">
         <v>-4.2325196307880697</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D64" s="13">
         <v>4.0668179433733697E-5</v>
       </c>
-      <c r="E64" t="s">
+      <c r="E64" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="8">
         <v>-6.9902044513956803</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65" s="13">
         <v>1.0139219425896501E-10</v>
       </c>
-      <c r="E65" t="s">
+      <c r="E65" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+      <c r="A66" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="8">
         <v>-7.1641374845187604</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66" s="13">
         <v>3.5025697870244099E-11</v>
       </c>
-      <c r="E66" t="s">
+      <c r="E66" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+      <c r="A67" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="8">
         <v>-5.70707673049818</v>
       </c>
-      <c r="D67" s="1">
+      <c r="D67" s="13">
         <v>6.6318331598363405E-8</v>
       </c>
-      <c r="E67" t="s">
+      <c r="E67" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="8">
         <v>-1.62849691511822</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="8">
         <v>0.105563054207653</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E68" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+      <c r="A69" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="8">
         <v>1.6981641830226999</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="8">
         <v>9.3288776504735493E-2</v>
       </c>
-      <c r="E69" t="s">
+      <c r="E69" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="8">
         <v>1.5734400688737999</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="8">
         <v>0.119716886786725</v>
       </c>
-      <c r="E70" t="s">
+      <c r="E70" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B71" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="11">
         <v>-1.18462108757482</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="11">
         <v>0.238423896474562</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E71" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B72" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="5">
         <v>-0.50770900200802704</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="5">
         <v>0.61245947183815297</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E72" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+      <c r="A73" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B73" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="8">
         <v>-5.0098036722115902</v>
       </c>
-      <c r="D73" s="1">
+      <c r="D73" s="13">
         <v>1.9603658479327199E-6</v>
       </c>
-      <c r="E73" t="s">
+      <c r="E73" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="A74" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B74" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="8">
         <v>-5.5280309140535104</v>
       </c>
-      <c r="D74" s="1">
+      <c r="D74" s="13">
         <v>2.7087121633269099E-7</v>
       </c>
-      <c r="E74" t="s">
+      <c r="E74" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+      <c r="A75" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="8">
         <v>-7.7186607183268396</v>
       </c>
-      <c r="D75" s="1">
+      <c r="D75" s="13">
         <v>1.73994034713175E-12</v>
       </c>
-      <c r="E75" t="s">
+      <c r="E75" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+      <c r="A76" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B76" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="8">
         <v>-1.9842129149132599</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="8">
         <v>4.9076700543837601E-2</v>
       </c>
-      <c r="E76" t="s">
+      <c r="E76" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="8">
         <v>-1.8127223880830099</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="8">
         <v>7.2603690018834099E-2</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="A78" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B78" t="s">
+      <c r="B78" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="8">
         <v>-2.51008662155435</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="8">
         <v>1.36787335556444E-2</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="A79" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B79" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="8">
         <v>0.57466662928852996</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="8">
         <v>0.56705311185201102</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B80" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="8">
         <v>0.29915245252171402</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="8">
         <v>0.76545866227643899</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="A81" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B81" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="11">
         <v>-1</v>
       </c>
-      <c r="D81">
+      <c r="D81" s="11">
         <v>0.319824461002787</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="5">
         <v>-1.30819201652872</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="5">
         <v>0.192998134907613</v>
       </c>
-      <c r="E82" t="s">
+      <c r="E82" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="A83" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C83">
+      <c r="C83" s="8">
         <v>-2.79433952125913</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="8">
         <v>5.9255124225659301E-3</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E83" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="A84" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C84">
+      <c r="C84" s="8">
         <v>-2.26109776503022</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="8">
         <v>2.5440467416266401E-2</v>
       </c>
-      <c r="E84" t="s">
+      <c r="E84" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="A85" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B85" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C85">
+      <c r="C85" s="8">
         <v>-2.1554583308806499</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="8">
         <v>3.3276871126874198E-2</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E85" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="A86" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B86" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C86">
+      <c r="C86" s="8">
         <v>0.54469938264678097</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="8">
         <v>0.58716000411325897</v>
       </c>
-      <c r="E86" t="s">
+      <c r="E86" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="A87" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B87" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C87">
+      <c r="C87" s="8">
         <v>0.559998179549965</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="8">
         <v>0.57675437142832198</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E87" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="A88" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B88" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C88">
+      <c r="C88" s="8">
         <v>0.94260355718632804</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="8">
         <v>0.34833826166826998</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E88" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="A89" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B89" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C89">
+      <c r="C89" s="8">
         <v>1.86508532811153</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="8">
         <v>6.5916959654828106E-2</v>
       </c>
-      <c r="E89" t="s">
+      <c r="E89" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="A90" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="8">
         <v>0.85561047371607102</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="8">
         <v>0.39432254554470297</v>
       </c>
-      <c r="E90" t="s">
+      <c r="E90" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="A91" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B91" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="11">
         <v>-0.936318303226778</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="11">
         <v>0.350643849388586</v>
       </c>
-      <c r="E91" t="s">
+      <c r="E91" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="A92" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B92" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C92">
+      <c r="C92" s="5">
         <v>-0.58434698333220902</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="5">
         <v>0.559883362436848</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E92" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="A93" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B93" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C93">
+      <c r="C93" s="8">
         <v>-2.4892999731070802</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="8">
         <v>1.3926430416939001E-2</v>
       </c>
-      <c r="E93" t="s">
+      <c r="E93" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="A94" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B94" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C94">
+      <c r="C94" s="8">
         <v>-1.7183192773588001</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="8">
         <v>8.8151327710138103E-2</v>
       </c>
-      <c r="E94" t="s">
+      <c r="E94" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="A95" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B95" t="s">
+      <c r="B95" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C95">
+      <c r="C95" s="8">
         <v>-2.9680962280408498</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="8">
         <v>3.5909267419618799E-3</v>
       </c>
-      <c r="E95" t="s">
+      <c r="E95" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="A96" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B96" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C96">
+      <c r="C96" s="8">
         <v>-0.82383886926121996</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="8">
         <v>0.41175436330961301</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E96" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="A97" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B97" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C97">
+      <c r="C97" s="8">
         <v>-0.337537520958818</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="8">
         <v>0.73622594488725601</v>
       </c>
-      <c r="E97" t="s">
+      <c r="E97" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="A98" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B98" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C98">
+      <c r="C98" s="8">
         <v>-0.73777165009569801</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="8">
         <v>0.46181485293010499</v>
       </c>
-      <c r="E98" t="s">
+      <c r="E98" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="A99" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B99" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="8">
         <v>1.5252079393326099</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="8">
         <v>0.131200839529482</v>
       </c>
-      <c r="E99" t="s">
+      <c r="E99" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="A100" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B100" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C100">
+      <c r="C100" s="8">
         <v>0.66953687657187499</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="8">
         <v>0.50472026474135201</v>
       </c>
-      <c r="E100" t="s">
+      <c r="E100" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="A101" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B101" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C101">
+      <c r="C101" s="11">
         <v>0.58096935247258696</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="11">
         <v>0.56297673168381102</v>
       </c>
-      <c r="E101" t="s">
+      <c r="E101" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="A102" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B102" t="s">
+      <c r="B102" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="5">
         <v>0.70282897871001304</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="5">
         <v>0.48390799171216298</v>
       </c>
-      <c r="E102" t="s">
+      <c r="E102" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="A103" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B103" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C103">
+      <c r="C103" s="8">
         <v>5.0999677241200096</v>
       </c>
-      <c r="D103" s="1">
+      <c r="D103" s="13">
         <v>3.11717715934499E-6</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E103" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="A104" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B104" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C104">
+      <c r="C104" s="8">
         <v>5.3426703769605099</v>
       </c>
-      <c r="D104" s="1">
+      <c r="D104" s="13">
         <v>1.29126073903671E-6</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E104" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="A105" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C105">
+      <c r="C105" s="8">
         <v>9.7625642329771996</v>
       </c>
-      <c r="D105" s="1">
+      <c r="D105" s="13">
         <v>4.9580250598145499E-17</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E105" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="A106" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C106">
+      <c r="C106" s="8">
         <v>5.7625304855120998</v>
       </c>
-      <c r="D106" s="1">
+      <c r="D106" s="13">
         <v>5.6596379058797902E-8</v>
       </c>
-      <c r="E106" t="s">
+      <c r="E106" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="A107" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B107" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C107">
+      <c r="C107" s="8">
         <v>5.6865488014549799</v>
       </c>
-      <c r="D107" s="1">
+      <c r="D107" s="13">
         <v>7.8634496483559305E-8</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E107" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="A108" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B108" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C108">
+      <c r="C108" s="8">
         <v>6.1242343189714497</v>
       </c>
-      <c r="D108" s="1">
+      <c r="D108" s="13">
         <v>9.4745902895293399E-9</v>
       </c>
-      <c r="E108" t="s">
+      <c r="E108" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="A109" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B109" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C109">
+      <c r="C109" s="8">
         <v>6.0177996593085004</v>
       </c>
-      <c r="D109" s="1">
+      <c r="D109" s="13">
         <v>3.0634417514815599E-8</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E109" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="A110" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B110" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C110">
+      <c r="C110" s="8">
         <v>0.16573422016345299</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="8">
         <v>0.86863913879329102</v>
       </c>
-      <c r="E110" t="s">
+      <c r="E110" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="A111" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C111">
+      <c r="C111" s="11">
         <v>-0.371695763671824</v>
       </c>
-      <c r="D111">
+      <c r="D111" s="11">
         <v>0.71082780074214502</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="A112" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B112" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C112">
+      <c r="C112" s="5">
         <v>-1.76316617922379</v>
       </c>
-      <c r="D112">
+      <c r="D112" s="5">
         <v>7.99216944952615E-2</v>
       </c>
-      <c r="E112" t="s">
+      <c r="E112" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="A113" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B113" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C113">
+      <c r="C113" s="8">
         <v>-4.6241633559446598</v>
       </c>
-      <c r="D113" s="1">
+      <c r="D113" s="13">
         <v>8.3181007905131992E-6</v>
       </c>
-      <c r="E113" t="s">
+      <c r="E113" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="A114" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B114" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C114">
+      <c r="C114" s="8">
         <v>-4.6701100576254504</v>
       </c>
-      <c r="D114" s="1">
+      <c r="D114" s="13">
         <v>6.9205800427501498E-6</v>
       </c>
-      <c r="E114" t="s">
+      <c r="E114" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="A115" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B115" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C115">
+      <c r="C115" s="8">
         <v>-5.22661474219053</v>
       </c>
-      <c r="D115" s="1">
+      <c r="D115" s="13">
         <v>8.2954933148744403E-7</v>
       </c>
-      <c r="E115" t="s">
+      <c r="E115" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="A116" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B116" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C116">
+      <c r="C116" s="8">
         <v>-2.0320218815131201</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="8">
         <v>4.42067393196919E-2</v>
       </c>
-      <c r="E116" t="s">
+      <c r="E116" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="A117" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C117">
+      <c r="C117" s="8">
         <v>-0.707526489736789</v>
       </c>
-      <c r="D117">
+      <c r="D117" s="8">
         <v>0.48046565214340398</v>
       </c>
-      <c r="E117" t="s">
+      <c r="E117" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="A118" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B118" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C118">
+      <c r="C118" s="8">
         <v>-1.17045680679894</v>
       </c>
-      <c r="D118">
+      <c r="D118" s="8">
         <v>0.24375838434776001</v>
       </c>
-      <c r="E118" t="s">
+      <c r="E118" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="A119" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B119" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C119">
+      <c r="C119" s="8">
         <v>0.52667171016619596</v>
       </c>
-      <c r="D119">
+      <c r="D119" s="8">
         <v>0.59953163196632298</v>
       </c>
-      <c r="E119" t="s">
+      <c r="E119" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="A120" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B120" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C120">
+      <c r="C120" s="8">
         <v>1.36983546822693</v>
       </c>
-      <c r="D120">
+      <c r="D120" s="8">
         <v>0.17404407847898901</v>
       </c>
-      <c r="E120" t="s">
+      <c r="E120" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="A121" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B121" t="s">
+      <c r="B121" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C121">
+      <c r="C121" s="11">
         <v>0.78576501502562601</v>
       </c>
-      <c r="D121">
+      <c r="D121" s="11">
         <v>0.43415353115927202</v>
       </c>
-      <c r="E121" t="s">
+      <c r="E121" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="A122" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C122">
+      <c r="C122" s="5">
         <v>-1.0281068746745401</v>
       </c>
-      <c r="D122">
+      <c r="D122" s="5">
         <v>0.30555219715482501</v>
       </c>
-      <c r="E122" t="s">
+      <c r="E122" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+      <c r="A123" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B123" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C123">
+      <c r="C123" s="8">
         <v>-3.3777345047543501</v>
       </c>
-      <c r="D123">
+      <c r="D123" s="8">
         <v>9.3004423270556401E-4</v>
       </c>
-      <c r="E123" t="s">
+      <c r="E123" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+      <c r="A124" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B124" t="s">
+      <c r="B124" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C124">
+      <c r="C124" s="8">
         <v>-2.6305526335452001</v>
       </c>
-      <c r="D124">
+      <c r="D124" s="8">
         <v>9.4398125384060894E-3</v>
       </c>
-      <c r="E124" t="s">
+      <c r="E124" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="A125" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B125" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C125">
+      <c r="C125" s="8">
         <v>-2.9064873374653302</v>
       </c>
-      <c r="D125">
+      <c r="D125" s="8">
         <v>4.3224127911205001E-3</v>
       </c>
-      <c r="E125" t="s">
+      <c r="E125" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="A126" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B126" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C126">
+      <c r="C126" s="8">
         <v>-1.27191544932939</v>
       </c>
-      <c r="D126">
+      <c r="D126" s="8">
         <v>0.20567352216828799</v>
       </c>
-      <c r="E126" t="s">
+      <c r="E126" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="A127" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B127" t="s">
+      <c r="B127" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C127">
+      <c r="C127" s="8">
         <v>-0.58056232965740795</v>
       </c>
-      <c r="D127">
+      <c r="D127" s="8">
         <v>0.56243338800380804</v>
       </c>
-      <c r="E127" t="s">
+      <c r="E127" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="A128" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B128" t="s">
+      <c r="B128" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C128">
+      <c r="C128" s="8">
         <v>-1.6203767520137999</v>
       </c>
-      <c r="D128">
+      <c r="D128" s="8">
         <v>0.10736781231959699</v>
       </c>
-      <c r="E128" t="s">
+      <c r="E128" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="A129" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C129">
+      <c r="C129" s="8">
         <v>1.3894667700211401</v>
       </c>
-      <c r="D129">
+      <c r="D129" s="8">
         <v>0.168456743759345</v>
       </c>
-      <c r="E129" t="s">
+      <c r="E129" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="A130" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C130">
+      <c r="C130" s="8">
         <v>1.2880314244344999</v>
       </c>
-      <c r="D130">
+      <c r="D130" s="8">
         <v>0.20131121664737101</v>
       </c>
-      <c r="E130" t="s">
+      <c r="E130" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="A131" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C131">
+      <c r="C131" s="11">
         <v>0.31770862894248802</v>
       </c>
-      <c r="D131">
+      <c r="D131" s="11">
         <v>0.75124535485730304</v>
       </c>
-      <c r="E131" t="s">
+      <c r="E131" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="A132" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C132">
+      <c r="C132" s="5">
         <v>-1.1031271259217601</v>
       </c>
-      <c r="D132">
+      <c r="D132" s="5">
         <v>0.271757032400817</v>
       </c>
-      <c r="E132" t="s">
+      <c r="E132" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="A133" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C133">
+      <c r="C133" s="8">
         <v>-4.1956301536406402</v>
       </c>
-      <c r="D133" s="1">
+      <c r="D133" s="13">
         <v>4.64621128465863E-5</v>
       </c>
-      <c r="E133" t="s">
+      <c r="E133" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="A134" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C134">
+      <c r="C134" s="8">
         <v>-3.9653165491965701</v>
       </c>
-      <c r="D134">
+      <c r="D134" s="8">
         <v>1.13427002195509E-4</v>
       </c>
-      <c r="E134" t="s">
+      <c r="E134" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="A135" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B135" t="s">
+      <c r="B135" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C135">
+      <c r="C135" s="8">
         <v>-4.57960452751992</v>
       </c>
-      <c r="D135" s="1">
+      <c r="D135" s="13">
         <v>1.00886335767195E-5</v>
       </c>
-      <c r="E135" t="s">
+      <c r="E135" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+      <c r="A136" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B136" t="s">
+      <c r="B136" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C136">
+      <c r="C136" s="8">
         <v>-2.1763045199223399</v>
       </c>
-      <c r="D136">
+      <c r="D136" s="8">
         <v>3.1235257813740099E-2</v>
       </c>
-      <c r="E136" t="s">
+      <c r="E136" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="A137" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C137">
+      <c r="C137" s="8">
         <v>-1.4321974072297501</v>
       </c>
-      <c r="D137">
+      <c r="D137" s="8">
         <v>0.154286287659223</v>
       </c>
-      <c r="E137" t="s">
+      <c r="E137" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="A138" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B138" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C138">
+      <c r="C138" s="8">
         <v>-0.84579741421460297</v>
       </c>
-      <c r="D138">
+      <c r="D138" s="8">
         <v>0.39910355591887903</v>
       </c>
-      <c r="E138" t="s">
+      <c r="E138" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="A139" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B139" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C139">
+      <c r="C139" s="8">
         <v>-0.45300094710049998</v>
       </c>
-      <c r="D139">
+      <c r="D139" s="8">
         <v>0.65137657638866198</v>
       </c>
-      <c r="E139" t="s">
+      <c r="E139" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="A140" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B140" t="s">
+      <c r="B140" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C140">
+      <c r="C140" s="8">
         <v>0.63719970874996601</v>
       </c>
-      <c r="D140">
+      <c r="D140" s="8">
         <v>0.52542968423615199</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E140" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="A141" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C141">
+      <c r="C141" s="11">
         <v>-0.341095951310598</v>
       </c>
-      <c r="D141">
+      <c r="D141" s="11">
         <v>0.73350648436812105</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E141" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+      <c r="A142" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C142">
+      <c r="C142" s="5">
         <v>-1.8081349008929799</v>
       </c>
-      <c r="D142">
+      <c r="D142" s="5">
         <v>7.3171066815877997E-2</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E142" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
+      <c r="A143" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C143">
+      <c r="C143" s="8">
         <v>-4.1506392570353903</v>
       </c>
-      <c r="D143" s="1">
+      <c r="D143" s="13">
         <v>5.5497966957093403E-5</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E143" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+      <c r="A144" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C144">
+      <c r="C144" s="8">
         <v>-3.94004958508875</v>
       </c>
-      <c r="D144">
+      <c r="D144" s="8">
         <v>1.2522082032290799E-4</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E144" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+      <c r="A145" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C145">
+      <c r="C145" s="8">
         <v>-3.0264534025583099</v>
       </c>
-      <c r="D145">
+      <c r="D145" s="8">
         <v>2.9734492193761002E-3</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E145" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
+      <c r="A146" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C146">
+      <c r="C146" s="8">
         <v>-0.63166355712483102</v>
       </c>
-      <c r="D146">
+      <c r="D146" s="8">
         <v>0.52885132633043397</v>
       </c>
-      <c r="E146" t="s">
+      <c r="E146" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
+      <c r="A147" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C147">
+      <c r="C147" s="8">
         <v>1.6386264529940999</v>
       </c>
-      <c r="D147">
+      <c r="D147" s="8">
         <v>0.10448794140493201</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E147" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
+      <c r="A148" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C148">
+      <c r="C148" s="8">
         <v>2.0240093902713499</v>
       </c>
-      <c r="D148">
+      <c r="D148" s="8">
         <v>4.5857894435142203E-2</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E148" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+      <c r="A149" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C149">
+      <c r="C149" s="8">
         <v>2.7360157072442002</v>
       </c>
-      <c r="D149">
+      <c r="D149" s="8">
         <v>7.68560863686037E-3</v>
       </c>
-      <c r="E149" t="s">
+      <c r="E149" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+      <c r="A150" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C150">
+      <c r="C150" s="8">
         <v>1.6955666146688</v>
       </c>
-      <c r="D150">
+      <c r="D150" s="8">
         <v>9.3519634132693194E-2</v>
       </c>
-      <c r="E150" t="s">
+      <c r="E150" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+      <c r="A151" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B151" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C151">
+      <c r="C151" s="11">
         <v>-1.2828797467709301</v>
       </c>
-      <c r="D151">
+      <c r="D151" s="11">
         <v>0.20213737615490601</v>
       </c>
-      <c r="E151" t="s">
+      <c r="E151" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
+      <c r="A152" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B152" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C152">
+      <c r="C152" s="5">
         <v>-1.0217210293724199</v>
       </c>
-      <c r="D152">
+      <c r="D152" s="5">
         <v>0.30871435029848798</v>
       </c>
-      <c r="E152" t="s">
+      <c r="E152" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
+      <c r="A153" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B153" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C153">
+      <c r="C153" s="8">
         <v>1.7216108445973399</v>
       </c>
-      <c r="D153">
+      <c r="D153" s="8">
         <v>8.9044631708431396E-2</v>
       </c>
-      <c r="E153" t="s">
+      <c r="E153" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
+      <c r="A154" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B154" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C154">
+      <c r="C154" s="8">
         <v>1.4596752865763001</v>
       </c>
-      <c r="D154">
+      <c r="D154" s="8">
         <v>0.148656439430711</v>
       </c>
-      <c r="E154" t="s">
+      <c r="E154" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+      <c r="A155" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B155" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C155">
+      <c r="C155" s="8">
         <v>1.9727601542469599</v>
       </c>
-      <c r="D155">
+      <c r="D155" s="8">
         <v>5.1584534994644403E-2</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E155" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+      <c r="A156" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B156" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C156">
+      <c r="C156" s="8">
         <v>0.146206002064663</v>
       </c>
-      <c r="D156">
+      <c r="D156" s="8">
         <v>0.884036892502711</v>
       </c>
-      <c r="E156" t="s">
+      <c r="E156" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
+      <c r="A157" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B157" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C157">
+      <c r="C157" s="8">
         <v>2.0218855737486501</v>
       </c>
-      <c r="D157">
+      <c r="D157" s="8">
         <v>4.6644974198876997E-2</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E157" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
+      <c r="A158" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C158">
+      <c r="C158" s="8">
         <v>2.0375574495698898</v>
       </c>
-      <c r="D158">
+      <c r="D158" s="8">
         <v>4.5024176615132999E-2</v>
       </c>
-      <c r="E158" t="s">
+      <c r="E158" s="9" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="A159" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C159">
+      <c r="C159" s="8">
         <v>3.9082098521657498</v>
       </c>
-      <c r="D159">
+      <c r="D159" s="8">
         <v>2.4548014461381698E-4</v>
       </c>
-      <c r="E159" t="s">
+      <c r="E159" s="9" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+      <c r="A160" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C160">
+      <c r="C160" s="8">
         <v>-1.95753908365463</v>
       </c>
-      <c r="D160">
+      <c r="D160" s="8">
         <v>5.3188021034275799E-2</v>
       </c>
-      <c r="E160" t="s">
+      <c r="E160" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
+      <c r="A161" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B161" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C161">
+      <c r="C161" s="11">
         <v>-0.85282825939548201</v>
       </c>
-      <c r="D161">
+      <c r="D161" s="11">
         <v>0.39568575948727203</v>
       </c>
-      <c r="E161" t="s">
+      <c r="E161" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
+      <c r="A162" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B162" t="s">
+      <c r="B162" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C162">
+      <c r="C162" s="5">
         <v>0.49339731237508799</v>
       </c>
-      <c r="D162">
+      <c r="D162" s="5">
         <v>0.62250462070244095</v>
       </c>
-      <c r="E162" t="s">
+      <c r="E162" s="6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
+      <c r="A163" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B163" t="s">
+      <c r="B163" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C163">
+      <c r="C163" s="8">
         <v>-0.48953467762549102</v>
       </c>
-      <c r="D163">
+      <c r="D163" s="8">
         <v>0.62532318550074095</v>
       </c>
-      <c r="E163" t="s">
+      <c r="E163" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="A164" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B164" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C164">
+      <c r="C164" s="8">
         <v>-1.3012604332575599</v>
       </c>
-      <c r="D164">
+      <c r="D164" s="8">
         <v>0.195153545216213</v>
       </c>
-      <c r="E164" t="s">
+      <c r="E164" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
+      <c r="A165" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B165" t="s">
+      <c r="B165" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C165">
+      <c r="C165" s="8">
         <v>-0.37507960843841498</v>
       </c>
-      <c r="D165">
+      <c r="D165" s="8">
         <v>0.70828027912801395</v>
       </c>
-      <c r="E165" t="s">
+      <c r="E165" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
+      <c r="A166" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B166" t="s">
+      <c r="B166" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C166">
+      <c r="C166" s="8">
         <v>1.64568479598705</v>
       </c>
-      <c r="D166">
+      <c r="D166" s="8">
         <v>0.105285068334192</v>
       </c>
-      <c r="E166" t="s">
+      <c r="E166" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
+      <c r="A167" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B167" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C167">
+      <c r="C167" s="8">
         <v>1.29520776455085</v>
       </c>
-      <c r="D167">
+      <c r="D167" s="8">
         <v>0.1997933154638</v>
       </c>
-      <c r="E167" t="s">
+      <c r="E167" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
+      <c r="A168" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B168" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C168">
+      <c r="C168" s="8">
         <v>0.81056867324352899</v>
       </c>
-      <c r="D168">
+      <c r="D168" s="8">
         <v>0.41991006134463899</v>
       </c>
-      <c r="E168" t="s">
+      <c r="E168" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
+      <c r="A169" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B169" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C169">
+      <c r="C169" s="8">
         <v>1.2145267692564701</v>
       </c>
-      <c r="D169">
+      <c r="D169" s="8">
         <v>0.228315812093071</v>
       </c>
-      <c r="E169" t="s">
+      <c r="E169" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
+      <c r="A170" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C170">
+      <c r="C170" s="8">
         <v>0.83665734013592097</v>
       </c>
-      <c r="D170">
+      <c r="D170" s="8">
         <v>0.40563107699185602</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
+      <c r="A171" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B171" t="s">
+      <c r="B171" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C171">
+      <c r="C171" s="11">
         <v>0.45482383254198799</v>
       </c>
-      <c r="D171">
+      <c r="D171" s="11">
         <v>0.650435004295569</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E171" s="12" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>